<commit_message>
added properties, testApp and documents (Aktivityplan)
</commit_message>
<xml_diff>
--- a/documents/06-Tagesberichte/Aufgabenverteilung.xlsx
+++ b/documents/06-Tagesberichte/Aufgabenverteilung.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Priv\Schule\git\Tante-Emma\documents\06-Tagesberichte\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="120" windowWidth="23715" windowHeight="9270"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Igor</t>
   </si>
@@ -31,9 +36,6 @@
   </si>
   <si>
     <t>Patrick</t>
-  </si>
-  <si>
-    <t>Scrum Modell</t>
   </si>
   <si>
     <t>Meilensteinplan</t>
@@ -233,14 +235,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -278,9 +283,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -315,7 +320,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,7 +355,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -524,11 +529,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,7 +548,7 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>0</v>
@@ -560,7 +565,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="14">
         <v>42858</v>
@@ -572,27 +577,27 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" s="13">
         <v>42865</v>
       </c>
       <c r="C3" s="11"/>
       <c r="D3" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -602,68 +607,66 @@
       <c r="B5" s="10">
         <v>42872</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>19</v>
+      </c>
       <c r="E5" s="11"/>
       <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="10">
-        <v>42872</v>
-      </c>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2">
+        <v>42879</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2">
         <v>42879</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B8" s="2">
-        <v>42879</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>20</v>
+        <v>42886</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="A9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="2">
-        <v>42886</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="14">
+        <v>42858</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
@@ -678,47 +681,49 @@
       <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="14">
-        <v>42858</v>
-      </c>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="B12" s="2">
+        <v>42865</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>24</v>
+      <c r="A13" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="B13" s="2">
-        <v>42865</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" s="2">
         <v>42940</v>
       </c>
     </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="10">
+        <v>42872</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="9" t="s">
+      <c r="A15" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="10">
-        <v>42872</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11" t="s">
-        <v>20</v>
+      <c r="B15" s="2">
+        <v>42879</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -728,11 +733,11 @@
       <c r="B16" s="2">
         <v>42879</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>20</v>
+      <c r="D16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -740,33 +745,30 @@
         <v>12</v>
       </c>
       <c r="B17" s="2">
-        <v>42879</v>
+        <v>42886</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18" s="2">
         <v>42886</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -774,10 +776,19 @@
         <v>15</v>
       </c>
       <c r="B19" s="2">
-        <v>42886</v>
+        <v>42879</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -788,49 +799,29 @@
         <v>42879</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="2">
-        <v>42879</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="10">
+      <c r="B21" s="10">
         <v>42872</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C21" s="11"/>
+      <c r="D21" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="11"/>
+      <c r="F21" s="11"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" t="s">
         <v>29</v>
-      </c>
-      <c r="B24" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>